<commit_message>
do manual computations of R
</commit_message>
<xml_diff>
--- a/data-raw/events.xlsx
+++ b/data-raw/events.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t xml:space="preserve">Significant Event Count::9</t>
   </si>
@@ -210,18 +210,25 @@
   </si>
   <si>
     <t xml:space="preserve">max I30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -324,7 +331,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,6 +421,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1241,9 +1252,9 @@
   <dimension ref="A1:AMJ230"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J190" activeCellId="0" sqref="J190"/>
+      <selection pane="bottomLeft" activeCell="K184" activeCellId="0" sqref="K184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,7 +1264,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,6 +1296,12 @@
       </c>
       <c r="I1" s="0" t="s">
         <v>61</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5579,9 +5598,13 @@
         <f aca="false">MAX(D118:D190)*2</f>
         <v>58.8</v>
       </c>
-      <c r="J190" s="0" t="n">
+      <c r="J190" s="23" t="n">
         <f aca="false">SUM(H118:H190)*I190</f>
         <v>630.238785903601</v>
+      </c>
+      <c r="K190" s="0" t="n">
+        <f aca="false">SUM(B118:B190)</f>
+        <v>46.4</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>